<commit_message>
Add generated Playwright test
</commit_message>
<xml_diff>
--- a/testmanager.xlsx
+++ b/testmanager.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,7 +562,7 @@
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E4" s="3" t="n"/>
@@ -759,7 +759,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E11" s="3" t="n">
@@ -916,6 +916,40 @@
         </is>
       </c>
       <c r="D16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Home Page validation UI</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Home Page validation UI</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test script for add new person</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>test script for add new person</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>